<commit_message>
updated for deployment & pr
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Amadeusalteajktmh07c2/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Amadeusalteajktmh07c2/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Amadeusalteajktmh07c2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76AA37D-239C-4B87-AB0E-59062E2AE745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D2F777-10E5-4187-B215-B80440C26874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21588" windowHeight="10584" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -185,9 +185,6 @@
     <t>PathSAKey</t>
   </si>
   <si>
-    <t>Captcha_RuleId</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -203,22 +200,22 @@
     <t>RPA_Moon_SenderName</t>
   </si>
   <si>
-    <t>RPA_Moon_Captcha_RuleId</t>
-  </si>
-  <si>
-    <t>RPA_Moon_GCaptcha_RuleId</t>
-  </si>
-  <si>
-    <t>GCaptcha_RuleId</t>
-  </si>
-  <si>
     <t>RPA_Moon_Cred_Gmail</t>
   </si>
   <si>
+    <t>RPA106_Air Asia_Email OTP</t>
+  </si>
+  <si>
+    <t>Cred_OTP</t>
+  </si>
+  <si>
+    <t>Cred email to get OTP</t>
+  </si>
+  <si>
     <t>RPA_Moon_UploadBucket</t>
   </si>
   <si>
-    <t>RPA_Moon_SheetIdConfig</t>
+    <t>RPA_Moon_SheetIdConfig_Transport</t>
   </si>
   <si>
     <t>RPA_Moon_PathMasterFolder</t>
@@ -234,15 +231,6 @@
   </si>
   <si>
     <t>RPA_Moon_DialogDownloadChrome</t>
-  </si>
-  <si>
-    <t>Cred_OTP</t>
-  </si>
-  <si>
-    <t>RPA106_Air Asia_Email OTP</t>
-  </si>
-  <si>
-    <t>Cred email to get OTP</t>
   </si>
 </sst>
 </file>
@@ -622,7 +610,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -669,10 +657,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -710,7 +698,7 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
@@ -718,13 +706,13 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2887,10 +2875,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -2942,7 +2930,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -2950,7 +2938,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -2958,7 +2946,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -2966,49 +2954,35 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3996,8 +3970,6 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>